<commit_message>
Update promo name in raffle promo excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/jchsCellphoneRaffleTicketClaim.xlsx
+++ b/src/main/resources/excel/jchsCellphoneRaffleTicketClaim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACF1B2C-EBEC-49DC-BA3F-624D1972F5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA6B6C-0694-4C0E-8DC1-C296E3927854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <t>TRANSACTION DATE</t>
   </si>
   <si>
-    <t>JCHS CELLPHONE RAFFLE</t>
+    <t>JCHS CELLPHONE RAFFLE PROMO</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Add Claim ID to Cellphone Raffle claim excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/jchsCellphoneRaffleTicketClaim.xlsx
+++ b/src/main/resources/excel/jchsCellphoneRaffleTicketClaim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJ\git\magic\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FA6B6C-0694-4C0E-8DC1-C296E3927854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56660B39-48F0-459A-8DEE-CD2ED7A62117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CUSTOMER CODE</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>JCHS CELLPHONE RAFFLE PROMO</t>
+  </si>
+  <si>
+    <t>CLAIM ID</t>
   </si>
 </sst>
 </file>
@@ -372,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -403,14 +406,19 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>